<commit_message>
addition of  Representation defined by the system Fixed Value: CMV Positive(#LA6576-8), Negative(#LA6577-6), Inconclusive(#LA11885-3), Invonclusive(#LA9663-1), Untested(#LA13538-6)
</commit_message>
<xml_diff>
--- a/StructureDefinition-ms-cmvgroup-observation.xlsx
+++ b/StructureDefinition-ms-cmvgroup-observation.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-01T13:56:53-05:00</t>
+    <t>2024-05-20T10:22:59-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -971,7 +971,7 @@
   &lt;coding&gt;
     &lt;system value="http://loinc.org"/&gt;
     &lt;code value="LA6576-8"/&gt;
-    &lt;display value="CMV Positive, Negative, Inconclusive, Invonclusive, Untested"/&gt;
+    &lt;display value="CMV Positive(#LA6576-8), Negative(#LA6577-6), Inconclusive(#LA11885-3), Invonclusive(#LA9663-1), Untested(#LA13538-6)"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>

</xml_diff>